<commit_message>
Fix SteeringServo constructor formatting and initialization
- Add space after comma in constructor parameter list for consistency
- Initialize current_steering_degree in constructor to match rest_position
- Update documentation
</commit_message>
<xml_diff>
--- a/Dokumentation.xlsx
+++ b/Dokumentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niklasschoning/Documents/Arduino/libraries/BuggyControl/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B05BF02-F61E-0444-A99A-7DD32E9F41B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF5425F-4009-7942-AAD1-F04B3EA5477F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{485CC123-1C10-6045-B34C-C7CEBDC1B1A4}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{485CC123-1C10-6045-B34C-C7CEBDC1B1A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Dokumentation BuggyControl Library
 -Niklas Schöning</t>
@@ -100,18 +100,6 @@
 gibt je nach type einen der Pins des Motors zurück</t>
   </si>
   <si>
-    <t>public bool changeSpeed(
-int direction_vector 
-)
-Diese Funktion sollte zum Ändern der Motorgeschwindigkeit als einzige direkt aufgerufen wird. Direction_vector ist die erwünschte Veränderung des Duty-Cycles/der Geschwindigkeit in %, kein absoluter Wert. Entscheidet anhand von threshhold, ob fadeDuty oder setDuty genutzt werden soll, initialisiert safetyDelay bei Richtungswechsel oder anhalten u.w.
-Gibt true zurück, falls nicht blockiert, sonst false</t>
-  </si>
-  <si>
-    <t>public bool checkDelay(
-)
-Wird von changeSpeed aufgerufen, um zu überprüfen, ob blockiert werden soll.</t>
-  </si>
-  <si>
     <t xml:space="preserve">LEDManager(
 std::vector&lt;int&gt; leds, //Liste aller LED-Pins, die der LED-Manager verwaltet
 int rest_state,  //Standard-verhalten der LEDs: 0 = aus, 1 = an
@@ -181,6 +169,34 @@
     <t>public int getSteeringDegree(
 )
 Gibt aktuellen Lenkwinkeln zurück</t>
+  </si>
+  <si>
+    <t>public void changeSpeed(
+int direction_vector 
+)
+Diese Funktion sollte zum Ändern der Motorgeschwindigkeit als einzige direkt aufgerufen wird. Direction_vector ist die erwünschte Veränderung des Duty-Cycles/der Geschwindigkeit in %, kein absoluter Wert. Entscheidet anhand von threshhold, ob fadeDuty oder setDuty genutzt werden soll, initialisiert safetyDelay bei Richtungswechsel oder anhalten u.w.</t>
+  </si>
+  <si>
+    <t>public void changeSpeedAbsolute(
+int target_duty
+)
+Ähnlich wie changeSpeed, aber setzt auf target_duty statt +- direction_vector</t>
+  </si>
+  <si>
+    <t>public int steer(
+int steering_vector
+)
+wird zum lenken aufgerufen, wechselt Lenkgrad um steering_vector(Delta in %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">public int steerAbsolute(
+int steering_degree
+)
+setzt den Lenkwinkel auf steering_degree(Absoluter Lenkwinkeln in %)
+</t>
+  </si>
+  <si>
+    <t>Anmerkung: Alle Prozentwerte haben eine Spanne von 100 bis -100 (steering_vector, direction_vector, steering_degree etc)</t>
   </si>
 </sst>
 </file>
@@ -201,7 +217,7 @@
       <name val="Aptos Narrow (Textkörper)"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -229,6 +245,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -260,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -274,10 +296,13 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -614,10 +639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBCC9135-BD93-8C43-8270-F2165723A60F}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -695,17 +720,17 @@
       </c>
       <c r="C9" s="6"/>
     </row>
-    <row r="10" spans="1:3" ht="170" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="153" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C10" s="6"/>
     </row>
     <row r="11" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="2" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C11" s="6"/>
     </row>
@@ -716,52 +741,52 @@
     </row>
     <row r="13" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C13" s="6"/>
     </row>
     <row r="14" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C14" s="6"/>
     </row>
     <row r="15" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C15" s="6"/>
     </row>
     <row r="16" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C16" s="6"/>
     </row>
     <row r="17" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C17" s="6"/>
     </row>
     <row r="18" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C18" s="6"/>
     </row>
     <row r="19" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C19" s="6"/>
     </row>
@@ -772,31 +797,50 @@
     </row>
     <row r="21" spans="1:3" ht="119" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="C21" s="6"/>
     </row>
-    <row r="22" spans="1:3" ht="102" x14ac:dyDescent="0.2">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2" t="s">
-        <v>23</v>
+    <row r="22" spans="1:3" ht="85" x14ac:dyDescent="0.2">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="C22" s="6"/>
     </row>
-    <row r="23" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C23" s="6"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
+    <row r="24" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="C24" s="6"/>
+    </row>
+    <row r="25" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="6"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+    </row>
+    <row r="27" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="B27" s="7" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>